<commit_message>
Eye level change to linear
</commit_message>
<xml_diff>
--- a/Projects/PNGAMERICA/Data/Template_v4.1.xlsx
+++ b/Projects/PNGAMERICA/Data/Template_v4.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="block and availability" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,21 +24,22 @@
     <sheet name="relative" sheetId="14" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$357</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">main!$A$1:$F$337</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -346,7 +347,7 @@
     <t>BLEACH AND LAUNDRY ADDITIVES</t>
   </si>
   <si>
-    <t>P&amp;G CATEGORY</t>
+    <t>PG_CATEGORY</t>
   </si>
   <si>
     <t>TOTAL FABRIC CONDITIONERS</t>
@@ -1039,7 +1040,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="82.8016194331984"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.5546558704453"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -1136,10 +1137,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="151.251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="152.538461538462"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1295,12 +1296,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.0931174089069"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="69.7327935222672"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1391,13 +1392,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="48.8461538461539"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.3117408906883"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.4939271255061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="49.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.7085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.2064777327935"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1568,9 +1569,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="102.728744939271"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="103.692307692308"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.7732793522267"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
@@ -1633,16 +1634,16 @@
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q5" activeCellId="0" sqref="Q5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.5222672064777"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1823,10 +1824,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="108.404858299595"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.1255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="109.368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.7692307692308"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.5951417004049"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2112,10 +2113,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="108.51012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="62.9878542510121"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.1295546558704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="109.473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.5222672064777"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="56.5587044534413"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2771,11 +2772,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.9068825910931"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="95.7651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -3522,12 +3523,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="153.931174089069"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="155.323886639676"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2793522267206"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -4875,15 +4876,15 @@
   </sheetPr>
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.1255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="83.8744939271255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="61.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3441295546559"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5159,9 +5160,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="102.728744939271"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.3441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="103.692307692308"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.0566801619433"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.7732793522267"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5617,10 +5618,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="120.400809716599"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.8461538461538"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="121.473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6006,10 +6007,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.7773279352227"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="102.728744939271"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="86.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="103.692307692308"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="87.1943319838057"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -12259,7 +12260,7 @@
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:F337"/>
+  <autoFilter ref="A1:F357"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>